<commit_message>
metagross def base stat
</commit_message>
<xml_diff>
--- a/national_pokedex.xlsx
+++ b/national_pokedex.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13864,124 +13864,10 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="91" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="92" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="149" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="150" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13990,28 +13876,28 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="138" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="139" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="146" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="147" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="86" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="73" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14026,28 +13912,52 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="142" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="143" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14056,40 +13966,94 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="144" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="103" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="145" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="104" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="107" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="105" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="108" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="106" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="93" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="94" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="102" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="148" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="96" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="97" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="87" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="88" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="90" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="91" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="92" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="113" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="109" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="110" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="111" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="112" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="115" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="116" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="117" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="118" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="114" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14098,28 +14062,52 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="122" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="78" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="123" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="81" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="124" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="125" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="135" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="119" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="120" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="121" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="126" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="127" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="128" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="136" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -14158,172 +14146,184 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="134" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="126" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="107" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="127" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="108" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="128" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="93" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="94" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="95" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="148" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="96" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="76" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="122" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="123" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="77" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="78" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="124" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="135" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="125" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="119" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="149" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="120" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="150" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="121" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="115" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="138" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="116" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="139" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="117" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="118" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="146" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="86" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="147" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="113" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="80" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="109" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="110" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="111" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="142" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="112" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="143" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="103" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="144" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="104" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="145" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="105" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="106" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="99" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="100" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="101" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="102" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="97" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="98" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="87" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="88" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="89" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="90" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="61" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="63" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="151" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15268,7 +15268,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15279,8 +15279,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AE810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="O177" sqref="O177"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="L377" sqref="L377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -15654,10 +15654,10 @@
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="M5" s="300" t="s">
+      <c r="M5" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="301"/>
+      <c r="N5" s="179"/>
       <c r="O5" s="2" t="s">
         <v>418</v>
       </c>
@@ -15729,10 +15729,10 @@
         <f t="shared" si="2"/>
         <v>129</v>
       </c>
-      <c r="M6" s="216" t="s">
+      <c r="M6" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="217"/>
+      <c r="N6" s="177"/>
       <c r="O6" s="2" t="s">
         <v>418</v>
       </c>
@@ -15896,10 +15896,10 @@
         <f t="shared" si="2"/>
         <v>122</v>
       </c>
-      <c r="M8" s="302" t="s">
+      <c r="M8" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="303"/>
+      <c r="N8" s="181"/>
       <c r="O8" s="2" t="s">
         <v>420</v>
       </c>
@@ -15971,10 +15971,10 @@
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-      <c r="M9" s="202" t="s">
+      <c r="M9" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="203"/>
+      <c r="N9" s="183"/>
       <c r="O9" s="2" t="s">
         <v>420</v>
       </c>
@@ -16046,10 +16046,10 @@
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="M10" s="202" t="s">
+      <c r="M10" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N10" s="203"/>
+      <c r="N10" s="183"/>
       <c r="O10" s="2" t="s">
         <v>420</v>
       </c>
@@ -16121,10 +16121,10 @@
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="M11" s="304" t="s">
+      <c r="M11" s="184" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="305"/>
+      <c r="N11" s="185"/>
       <c r="O11" s="2" t="s">
         <v>421</v>
       </c>
@@ -16196,10 +16196,10 @@
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
-      <c r="M12" s="234" t="s">
+      <c r="M12" s="260" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="235"/>
+      <c r="N12" s="261"/>
       <c r="O12" s="2" t="s">
         <v>421</v>
       </c>
@@ -16830,10 +16830,10 @@
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="M20" s="200" t="s">
+      <c r="M20" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="201"/>
+      <c r="N20" s="163"/>
       <c r="O20" s="2" t="s">
         <v>425</v>
       </c>
@@ -16905,10 +16905,10 @@
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="M21" s="200" t="s">
+      <c r="M21" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N21" s="201"/>
+      <c r="N21" s="163"/>
       <c r="O21" s="2" t="s">
         <v>425</v>
       </c>
@@ -17144,10 +17144,10 @@
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
-      <c r="M24" s="228" t="s">
+      <c r="M24" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="229"/>
+      <c r="N24" s="161"/>
       <c r="O24" s="2" t="s">
         <v>426</v>
       </c>
@@ -17224,10 +17224,10 @@
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="M25" s="228" t="s">
+      <c r="M25" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N25" s="229"/>
+      <c r="N25" s="161"/>
       <c r="O25" s="2" t="s">
         <v>426</v>
       </c>
@@ -17299,10 +17299,10 @@
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
-      <c r="M26" s="312" t="s">
+      <c r="M26" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="N26" s="313"/>
+      <c r="N26" s="165"/>
       <c r="O26" s="2" t="s">
         <v>427</v>
       </c>
@@ -17379,10 +17379,10 @@
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="M27" s="306" t="s">
+      <c r="M27" s="186" t="s">
         <v>18</v>
       </c>
-      <c r="N27" s="307"/>
+      <c r="N27" s="187"/>
       <c r="O27" s="2" t="s">
         <v>427</v>
       </c>
@@ -17464,10 +17464,10 @@
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
-      <c r="M28" s="308" t="s">
+      <c r="M28" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="N28" s="309"/>
+      <c r="N28" s="189"/>
       <c r="O28" s="2" t="s">
         <v>428</v>
       </c>
@@ -17544,10 +17544,10 @@
         <f t="shared" si="2"/>
         <v>202</v>
       </c>
-      <c r="M29" s="310" t="s">
+      <c r="M29" s="190" t="s">
         <v>19</v>
       </c>
-      <c r="N29" s="311"/>
+      <c r="N29" s="191"/>
       <c r="O29" s="2" t="s">
         <v>428</v>
       </c>
@@ -17619,10 +17619,10 @@
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
-      <c r="M30" s="228" t="s">
+      <c r="M30" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="229"/>
+      <c r="N30" s="161"/>
       <c r="O30" s="2" t="s">
         <v>426</v>
       </c>
@@ -17694,10 +17694,10 @@
         <f t="shared" si="2"/>
         <v>126</v>
       </c>
-      <c r="M31" s="228" t="s">
+      <c r="M31" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N31" s="229"/>
+      <c r="N31" s="161"/>
       <c r="O31" s="2" t="s">
         <v>426</v>
       </c>
@@ -17846,10 +17846,10 @@
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="M33" s="228" t="s">
+      <c r="M33" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N33" s="229"/>
+      <c r="N33" s="161"/>
       <c r="O33" s="2" t="s">
         <v>426</v>
       </c>
@@ -17921,10 +17921,10 @@
         <f t="shared" si="2"/>
         <v>112</v>
       </c>
-      <c r="M34" s="228" t="s">
+      <c r="M34" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N34" s="229"/>
+      <c r="N34" s="161"/>
       <c r="O34" s="2" t="s">
         <v>426</v>
       </c>
@@ -18078,10 +18078,10 @@
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="M36" s="210" t="s">
+      <c r="M36" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N36" s="211"/>
+      <c r="N36" s="173"/>
       <c r="O36" s="2" t="s">
         <v>568</v>
       </c>
@@ -18153,10 +18153,10 @@
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
-      <c r="M37" s="212" t="s">
+      <c r="M37" s="174" t="s">
         <v>30</v>
       </c>
-      <c r="N37" s="213"/>
+      <c r="N37" s="175"/>
       <c r="O37" s="2" t="s">
         <v>568</v>
       </c>
@@ -18233,10 +18233,10 @@
         <f t="shared" si="2"/>
         <v>122</v>
       </c>
-      <c r="M38" s="216" t="s">
+      <c r="M38" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N38" s="217"/>
+      <c r="N38" s="177"/>
       <c r="O38" s="2" t="s">
         <v>418</v>
       </c>
@@ -18308,10 +18308,10 @@
         <f t="shared" si="2"/>
         <v>204</v>
       </c>
-      <c r="M39" s="216" t="s">
+      <c r="M39" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N39" s="217"/>
+      <c r="N39" s="177"/>
       <c r="O39" s="2" t="s">
         <v>418</v>
       </c>
@@ -19270,10 +19270,10 @@
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="M51" s="240" t="s">
+      <c r="M51" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="N51" s="241"/>
+      <c r="N51" s="167"/>
       <c r="O51" s="2" t="s">
         <v>428</v>
       </c>
@@ -19350,10 +19350,10 @@
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
-      <c r="M52" s="242" t="s">
+      <c r="M52" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="N52" s="243"/>
+      <c r="N52" s="169"/>
       <c r="O52" s="2" t="s">
         <v>428</v>
       </c>
@@ -19430,10 +19430,10 @@
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
-      <c r="M53" s="200" t="s">
+      <c r="M53" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N53" s="201"/>
+      <c r="N53" s="163"/>
       <c r="O53" s="2" t="s">
         <v>425</v>
       </c>
@@ -19510,10 +19510,10 @@
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
-      <c r="M54" s="278" t="s">
+      <c r="M54" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="N54" s="279"/>
+      <c r="N54" s="171"/>
       <c r="O54" s="2" t="s">
         <v>425</v>
       </c>
@@ -19590,10 +19590,10 @@
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="M55" s="202" t="s">
+      <c r="M55" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N55" s="203"/>
+      <c r="N55" s="183"/>
       <c r="O55" s="2" t="s">
         <v>420</v>
       </c>
@@ -19665,10 +19665,10 @@
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
-      <c r="M56" s="296" t="s">
+      <c r="M56" s="208" t="s">
         <v>15</v>
       </c>
-      <c r="N56" s="297"/>
+      <c r="N56" s="209"/>
       <c r="O56" s="2" t="s">
         <v>420</v>
       </c>
@@ -19740,10 +19740,10 @@
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="M57" s="192" t="s">
+      <c r="M57" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N57" s="193"/>
+      <c r="N57" s="207"/>
       <c r="O57" s="2" t="s">
         <v>432</v>
       </c>
@@ -19815,10 +19815,10 @@
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="M58" s="192" t="s">
+      <c r="M58" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N58" s="193"/>
+      <c r="N58" s="207"/>
       <c r="O58" s="2" t="s">
         <v>432</v>
       </c>
@@ -19900,10 +19900,10 @@
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="M59" s="298" t="s">
+      <c r="M59" s="210" t="s">
         <v>13</v>
       </c>
-      <c r="N59" s="299"/>
+      <c r="N59" s="211"/>
       <c r="O59" s="2" t="s">
         <v>418</v>
       </c>
@@ -19975,10 +19975,10 @@
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
-      <c r="M60" s="216" t="s">
+      <c r="M60" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N60" s="217"/>
+      <c r="N60" s="177"/>
       <c r="O60" s="2" t="s">
         <v>418</v>
       </c>
@@ -20060,10 +20060,10 @@
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="M61" s="194" t="s">
+      <c r="M61" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="N61" s="195"/>
+      <c r="N61" s="213"/>
       <c r="O61" s="2" t="s">
         <v>420</v>
       </c>
@@ -20135,10 +20135,10 @@
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="M62" s="230" t="s">
+      <c r="M62" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="N62" s="231"/>
+      <c r="N62" s="257"/>
       <c r="O62" s="2" t="s">
         <v>420</v>
       </c>
@@ -20302,10 +20302,10 @@
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-      <c r="M64" s="262" t="s">
+      <c r="M64" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="N64" s="263"/>
+      <c r="N64" s="203"/>
       <c r="O64" s="2" t="s">
         <v>434</v>
       </c>
@@ -20377,10 +20377,10 @@
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="M65" s="222" t="s">
+      <c r="M65" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="N65" s="223"/>
+      <c r="N65" s="193"/>
       <c r="O65" s="2" t="s">
         <v>434</v>
       </c>
@@ -20452,10 +20452,10 @@
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-      <c r="M66" s="294" t="s">
+      <c r="M66" s="204" t="s">
         <v>21</v>
       </c>
-      <c r="N66" s="295"/>
+      <c r="N66" s="205"/>
       <c r="O66" s="2" t="s">
         <v>434</v>
       </c>
@@ -20532,10 +20532,10 @@
         <f t="shared" ref="L67:L130" si="5">ROUND((1+(H67-75)/500)*(ROUND(0.25*(7*MAX(G67,E67)+MIN(G67,E67)),0)),0)</f>
         <v>88</v>
       </c>
-      <c r="M67" s="192" t="s">
+      <c r="M67" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N67" s="193"/>
+      <c r="N67" s="207"/>
       <c r="O67" s="2" t="s">
         <v>432</v>
       </c>
@@ -20612,10 +20612,10 @@
         <f t="shared" si="5"/>
         <v>130</v>
       </c>
-      <c r="M68" s="192" t="s">
+      <c r="M68" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N68" s="193"/>
+      <c r="N68" s="207"/>
       <c r="O68" s="2" t="s">
         <v>432</v>
       </c>
@@ -20692,10 +20692,10 @@
         <f t="shared" si="5"/>
         <v>162</v>
       </c>
-      <c r="M69" s="192" t="s">
+      <c r="M69" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N69" s="193"/>
+      <c r="N69" s="207"/>
       <c r="O69" s="2" t="s">
         <v>432</v>
       </c>
@@ -21418,10 +21418,10 @@
         <f t="shared" si="5"/>
         <v>132</v>
       </c>
-      <c r="M78" s="216" t="s">
+      <c r="M78" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N78" s="217"/>
+      <c r="N78" s="177"/>
       <c r="O78" s="2" t="s">
         <v>418</v>
       </c>
@@ -21498,10 +21498,10 @@
         <f t="shared" si="5"/>
         <v>167</v>
       </c>
-      <c r="M79" s="290" t="s">
+      <c r="M79" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="N79" s="291"/>
+      <c r="N79" s="199"/>
       <c r="O79" s="2" t="s">
         <v>418</v>
       </c>
@@ -22142,10 +22142,10 @@
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="M87" s="202" t="s">
+      <c r="M87" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N87" s="203"/>
+      <c r="N87" s="183"/>
       <c r="O87" s="2" t="s">
         <v>420</v>
       </c>
@@ -22314,10 +22314,10 @@
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
-      <c r="M89" s="228" t="s">
+      <c r="M89" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N89" s="229"/>
+      <c r="N89" s="161"/>
       <c r="O89" s="2" t="s">
         <v>426</v>
       </c>
@@ -22394,10 +22394,10 @@
         <f t="shared" si="5"/>
         <v>184</v>
       </c>
-      <c r="M90" s="228" t="s">
+      <c r="M90" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N90" s="229"/>
+      <c r="N90" s="161"/>
       <c r="O90" s="2" t="s">
         <v>426</v>
       </c>
@@ -22474,10 +22474,10 @@
         <f t="shared" si="5"/>
         <v>168</v>
       </c>
-      <c r="M91" s="292" t="s">
+      <c r="M91" s="200" t="s">
         <v>15</v>
       </c>
-      <c r="N91" s="293"/>
+      <c r="N91" s="201"/>
       <c r="O91" s="2" t="s">
         <v>420</v>
       </c>
@@ -22974,10 +22974,10 @@
         <f t="shared" si="5"/>
         <v>158</v>
       </c>
-      <c r="M97" s="222" t="s">
+      <c r="M97" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="N97" s="223"/>
+      <c r="N97" s="193"/>
       <c r="O97" s="2" t="s">
         <v>434</v>
       </c>
@@ -23049,10 +23049,10 @@
         <f t="shared" si="5"/>
         <v>215</v>
       </c>
-      <c r="M98" s="222" t="s">
+      <c r="M98" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="N98" s="223"/>
+      <c r="N98" s="193"/>
       <c r="O98" s="2" t="s">
         <v>434</v>
       </c>
@@ -23129,10 +23129,10 @@
         <f t="shared" si="5"/>
         <v>156</v>
       </c>
-      <c r="M99" s="286" t="s">
+      <c r="M99" s="194" t="s">
         <v>15</v>
       </c>
-      <c r="N99" s="287"/>
+      <c r="N99" s="195"/>
       <c r="O99" s="2" t="s">
         <v>420</v>
       </c>
@@ -23204,10 +23204,10 @@
         <f t="shared" si="5"/>
         <v>214</v>
       </c>
-      <c r="M100" s="202" t="s">
+      <c r="M100" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N100" s="203"/>
+      <c r="N100" s="183"/>
       <c r="O100" s="2" t="s">
         <v>420</v>
       </c>
@@ -23284,10 +23284,10 @@
         <f t="shared" si="5"/>
         <v>114</v>
       </c>
-      <c r="M101" s="288" t="s">
+      <c r="M101" s="196" t="s">
         <v>18</v>
       </c>
-      <c r="N101" s="289"/>
+      <c r="N101" s="197"/>
       <c r="O101" s="2" t="s">
         <v>427</v>
       </c>
@@ -23364,10 +23364,10 @@
         <f t="shared" si="5"/>
         <v>179</v>
       </c>
-      <c r="M102" s="226" t="s">
+      <c r="M102" s="254" t="s">
         <v>18</v>
       </c>
-      <c r="N102" s="227"/>
+      <c r="N102" s="255"/>
       <c r="O102" s="2" t="s">
         <v>427</v>
       </c>
@@ -23603,10 +23603,10 @@
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="M105" s="240" t="s">
+      <c r="M105" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="N105" s="241"/>
+      <c r="N105" s="167"/>
       <c r="O105" s="2" t="s">
         <v>428</v>
       </c>
@@ -23678,10 +23678,10 @@
         <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="M106" s="282" t="s">
+      <c r="M106" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="N106" s="283"/>
+      <c r="N106" s="217"/>
       <c r="O106" s="2" t="s">
         <v>428</v>
       </c>
@@ -23753,10 +23753,10 @@
         <f t="shared" si="5"/>
         <v>211</v>
       </c>
-      <c r="M107" s="192" t="s">
+      <c r="M107" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N107" s="193"/>
+      <c r="N107" s="207"/>
       <c r="O107" s="2" t="s">
         <v>432</v>
       </c>
@@ -23833,10 +23833,10 @@
         <f t="shared" si="5"/>
         <v>212</v>
       </c>
-      <c r="M108" s="192" t="s">
+      <c r="M108" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N108" s="193"/>
+      <c r="N108" s="207"/>
       <c r="O108" s="2" t="s">
         <v>432</v>
       </c>
@@ -23918,10 +23918,10 @@
         <f t="shared" si="5"/>
         <v>137</v>
       </c>
-      <c r="M109" s="284" t="s">
+      <c r="M109" s="218" t="s">
         <v>17</v>
       </c>
-      <c r="N109" s="285"/>
+      <c r="N109" s="219"/>
       <c r="O109" s="2" t="s">
         <v>425</v>
       </c>
@@ -23993,10 +23993,10 @@
         <f t="shared" si="5"/>
         <v>164</v>
       </c>
-      <c r="M110" s="228" t="s">
+      <c r="M110" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N110" s="229"/>
+      <c r="N110" s="161"/>
       <c r="O110" s="2" t="s">
         <v>426</v>
       </c>
@@ -24073,10 +24073,10 @@
         <f t="shared" si="5"/>
         <v>221</v>
       </c>
-      <c r="M111" s="228" t="s">
+      <c r="M111" s="160" t="s">
         <v>12</v>
       </c>
-      <c r="N111" s="229"/>
+      <c r="N111" s="161"/>
       <c r="O111" s="2" t="s">
         <v>426</v>
       </c>
@@ -24312,10 +24312,10 @@
         <f t="shared" si="5"/>
         <v>176</v>
       </c>
-      <c r="M114" s="210" t="s">
+      <c r="M114" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N114" s="211"/>
+      <c r="N114" s="173"/>
       <c r="O114" s="2" t="s">
         <v>425</v>
       </c>
@@ -24392,10 +24392,10 @@
         <f t="shared" si="5"/>
         <v>205</v>
       </c>
-      <c r="M115" s="280" t="s">
+      <c r="M115" s="214" t="s">
         <v>11</v>
       </c>
-      <c r="N115" s="281"/>
+      <c r="N115" s="215"/>
       <c r="O115" s="2" t="s">
         <v>443</v>
       </c>
@@ -24472,10 +24472,10 @@
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="M116" s="278" t="s">
+      <c r="M116" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="N116" s="279"/>
+      <c r="N116" s="171"/>
       <c r="O116" s="2" t="s">
         <v>425</v>
       </c>
@@ -24552,10 +24552,10 @@
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="M117" s="202" t="s">
+      <c r="M117" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N117" s="203"/>
+      <c r="N117" s="183"/>
       <c r="O117" s="2" t="s">
         <v>420</v>
       </c>
@@ -24627,10 +24627,10 @@
         <f t="shared" si="5"/>
         <v>182</v>
       </c>
-      <c r="M118" s="202" t="s">
+      <c r="M118" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N118" s="203"/>
+      <c r="N118" s="183"/>
       <c r="O118" s="2" t="s">
         <v>420</v>
       </c>
@@ -24707,10 +24707,10 @@
         <f t="shared" si="5"/>
         <v>115</v>
       </c>
-      <c r="M119" s="202" t="s">
+      <c r="M119" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N119" s="203"/>
+      <c r="N119" s="183"/>
       <c r="O119" s="2" t="s">
         <v>420</v>
       </c>
@@ -24782,10 +24782,10 @@
         <f t="shared" si="5"/>
         <v>154</v>
       </c>
-      <c r="M120" s="202" t="s">
+      <c r="M120" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N120" s="203"/>
+      <c r="N120" s="183"/>
       <c r="O120" s="2" t="s">
         <v>420</v>
       </c>
@@ -24867,10 +24867,10 @@
         <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="M121" s="230" t="s">
+      <c r="M121" s="256" t="s">
         <v>15</v>
       </c>
-      <c r="N121" s="231"/>
+      <c r="N121" s="257"/>
       <c r="O121" s="96" t="s">
         <v>3494</v>
       </c>
@@ -25285,10 +25285,10 @@
         <f t="shared" si="5"/>
         <v>173</v>
       </c>
-      <c r="M126" s="236" t="s">
+      <c r="M126" s="224" t="s">
         <v>18</v>
       </c>
-      <c r="N126" s="237"/>
+      <c r="N126" s="225"/>
       <c r="O126" s="2" t="s">
         <v>427</v>
       </c>
@@ -25360,10 +25360,10 @@
         <f t="shared" si="5"/>
         <v>169</v>
       </c>
-      <c r="M127" s="216" t="s">
+      <c r="M127" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N127" s="217"/>
+      <c r="N127" s="177"/>
       <c r="O127" s="2" t="s">
         <v>418</v>
       </c>
@@ -25435,10 +25435,10 @@
         <f t="shared" si="5"/>
         <v>197</v>
       </c>
-      <c r="M128" s="274" t="s">
+      <c r="M128" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="N128" s="275"/>
+      <c r="N128" s="221"/>
       <c r="O128" s="2" t="s">
         <v>421</v>
       </c>
@@ -25520,10 +25520,10 @@
         <f t="shared" si="5"/>
         <v>197</v>
       </c>
-      <c r="M129" s="276" t="s">
+      <c r="M129" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="N129" s="277"/>
+      <c r="N129" s="223"/>
       <c r="O129" s="2" t="s">
         <v>425</v>
       </c>
@@ -25595,10 +25595,10 @@
         <f t="shared" si="5"/>
         <v>102</v>
       </c>
-      <c r="M130" s="202" t="s">
+      <c r="M130" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N130" s="203"/>
+      <c r="N130" s="183"/>
       <c r="O130" s="2" t="s">
         <v>420</v>
       </c>
@@ -25844,10 +25844,10 @@
         <f t="shared" si="8"/>
         <v>91</v>
       </c>
-      <c r="M133" s="210" t="s">
+      <c r="M133" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N133" s="211"/>
+      <c r="N133" s="173"/>
       <c r="O133" s="2" t="s">
         <v>425</v>
       </c>
@@ -25919,10 +25919,10 @@
         <f t="shared" si="8"/>
         <v>121</v>
       </c>
-      <c r="M134" s="278" t="s">
+      <c r="M134" s="170" t="s">
         <v>17</v>
       </c>
-      <c r="N134" s="279"/>
+      <c r="N134" s="171"/>
       <c r="O134" s="2" t="s">
         <v>425</v>
       </c>
@@ -25999,10 +25999,10 @@
         <f t="shared" si="8"/>
         <v>177</v>
       </c>
-      <c r="M135" s="202" t="s">
+      <c r="M135" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N135" s="203"/>
+      <c r="N135" s="183"/>
       <c r="O135" s="2" t="s">
         <v>420</v>
       </c>
@@ -26074,10 +26074,10 @@
         <f t="shared" si="8"/>
         <v>201</v>
       </c>
-      <c r="M136" s="270" t="s">
+      <c r="M136" s="232" t="s">
         <v>18</v>
       </c>
-      <c r="N136" s="271"/>
+      <c r="N136" s="233"/>
       <c r="O136" s="2" t="s">
         <v>427</v>
       </c>
@@ -26149,10 +26149,10 @@
         <f t="shared" si="8"/>
         <v>204</v>
       </c>
-      <c r="M137" s="216" t="s">
+      <c r="M137" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N137" s="217"/>
+      <c r="N137" s="177"/>
       <c r="O137" s="2" t="s">
         <v>418</v>
       </c>
@@ -26229,10 +26229,10 @@
         <f t="shared" si="8"/>
         <v>139</v>
       </c>
-      <c r="M138" s="272" t="s">
+      <c r="M138" s="236" t="s">
         <v>17</v>
       </c>
-      <c r="N138" s="273"/>
+      <c r="N138" s="237"/>
       <c r="O138" s="2" t="s">
         <v>425</v>
       </c>
@@ -26719,10 +26719,10 @@
         <f t="shared" si="8"/>
         <v>190</v>
       </c>
-      <c r="M144" s="210" t="s">
+      <c r="M144" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N144" s="211"/>
+      <c r="N144" s="173"/>
       <c r="O144" s="2" t="s">
         <v>425</v>
       </c>
@@ -27050,10 +27050,10 @@
         <f t="shared" si="8"/>
         <v>94</v>
       </c>
-      <c r="M148" s="198" t="s">
+      <c r="M148" s="234" t="s">
         <v>26</v>
       </c>
-      <c r="N148" s="199"/>
+      <c r="N148" s="235"/>
       <c r="O148" s="2" t="s">
         <v>450</v>
       </c>
@@ -27125,10 +27125,10 @@
         <f t="shared" si="8"/>
         <v>138</v>
       </c>
-      <c r="M149" s="198" t="s">
+      <c r="M149" s="234" t="s">
         <v>26</v>
       </c>
-      <c r="N149" s="199"/>
+      <c r="N149" s="235"/>
       <c r="O149" s="2" t="s">
         <v>450</v>
       </c>
@@ -27284,10 +27284,10 @@
       <c r="L151" s="2">
         <v>182</v>
       </c>
-      <c r="M151" s="262" t="s">
+      <c r="M151" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="N151" s="263"/>
+      <c r="N151" s="203"/>
       <c r="O151" s="2" t="s">
         <v>434</v>
       </c>
@@ -27359,10 +27359,10 @@
         <f t="shared" si="8"/>
         <v>210</v>
       </c>
-      <c r="M152" s="222" t="s">
+      <c r="M152" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="N152" s="223"/>
+      <c r="N152" s="193"/>
       <c r="O152" s="2" t="s">
         <v>434</v>
       </c>
@@ -27439,10 +27439,10 @@
         <f t="shared" si="8"/>
         <v>122</v>
       </c>
-      <c r="M153" s="264" t="s">
+      <c r="M153" s="226" t="s">
         <v>11</v>
       </c>
-      <c r="N153" s="265"/>
+      <c r="N153" s="227"/>
       <c r="O153" s="2" t="s">
         <v>443</v>
       </c>
@@ -27512,10 +27512,10 @@
         <f t="shared" si="8"/>
         <v>155</v>
       </c>
-      <c r="M154" s="266" t="s">
+      <c r="M154" s="228" t="s">
         <v>11</v>
       </c>
-      <c r="N154" s="267"/>
+      <c r="N154" s="229"/>
       <c r="O154" s="2" t="s">
         <v>443</v>
       </c>
@@ -27585,10 +27585,10 @@
         <f t="shared" si="8"/>
         <v>202</v>
       </c>
-      <c r="M155" s="268" t="s">
+      <c r="M155" s="230" t="s">
         <v>11</v>
       </c>
-      <c r="N155" s="269"/>
+      <c r="N155" s="231"/>
       <c r="O155" s="2" t="s">
         <v>443</v>
       </c>
@@ -27658,10 +27658,10 @@
         <f t="shared" si="8"/>
         <v>96</v>
       </c>
-      <c r="M156" s="216" t="s">
+      <c r="M156" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N156" s="217"/>
+      <c r="N156" s="177"/>
       <c r="O156" s="2" t="s">
         <v>418</v>
       </c>
@@ -27731,10 +27731,10 @@
         <f t="shared" si="8"/>
         <v>129</v>
       </c>
-      <c r="M157" s="216" t="s">
+      <c r="M157" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N157" s="217"/>
+      <c r="N157" s="177"/>
       <c r="O157" s="2" t="s">
         <v>418</v>
       </c>
@@ -27804,10 +27804,10 @@
         <f t="shared" si="8"/>
         <v>176</v>
       </c>
-      <c r="M158" s="216" t="s">
+      <c r="M158" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N158" s="217"/>
+      <c r="N158" s="177"/>
       <c r="O158" s="2" t="s">
         <v>418</v>
       </c>
@@ -27877,10 +27877,10 @@
         <f t="shared" si="8"/>
         <v>116</v>
       </c>
-      <c r="M159" s="194" t="s">
+      <c r="M159" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="N159" s="195"/>
+      <c r="N159" s="213"/>
       <c r="O159" s="2" t="s">
         <v>420</v>
       </c>
@@ -27950,10 +27950,10 @@
         <f t="shared" si="8"/>
         <v>151</v>
       </c>
-      <c r="M160" s="202" t="s">
+      <c r="M160" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N160" s="203"/>
+      <c r="N160" s="183"/>
       <c r="O160" s="2" t="s">
         <v>420</v>
       </c>
@@ -28023,10 +28023,10 @@
         <f t="shared" si="8"/>
         <v>197</v>
       </c>
-      <c r="M161" s="202" t="s">
+      <c r="M161" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N161" s="203"/>
+      <c r="N161" s="183"/>
       <c r="O161" s="2" t="s">
         <v>420</v>
       </c>
@@ -28102,10 +28102,10 @@
         <f t="shared" si="8"/>
         <v>77</v>
       </c>
-      <c r="M162" s="258" t="s">
+      <c r="M162" s="238" t="s">
         <v>17</v>
       </c>
-      <c r="N162" s="259"/>
+      <c r="N162" s="239"/>
       <c r="O162" s="2" t="s">
         <v>425</v>
       </c>
@@ -28175,10 +28175,10 @@
         <f t="shared" si="8"/>
         <v>130</v>
       </c>
-      <c r="M163" s="200" t="s">
+      <c r="M163" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N163" s="201"/>
+      <c r="N163" s="163"/>
       <c r="O163" s="2" t="s">
         <v>425</v>
       </c>
@@ -28923,10 +28923,10 @@
         <f t="shared" si="8"/>
         <v>63</v>
       </c>
-      <c r="M173" s="260" t="s">
+      <c r="M173" s="240" t="s">
         <v>18</v>
       </c>
-      <c r="N173" s="261"/>
+      <c r="N173" s="241"/>
       <c r="O173" s="2" t="s">
         <v>427</v>
       </c>
@@ -29002,10 +29002,10 @@
         <f t="shared" si="8"/>
         <v>91</v>
       </c>
-      <c r="M174" s="200" t="s">
+      <c r="M174" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="N174" s="201"/>
+      <c r="N174" s="163"/>
       <c r="O174" s="2" t="s">
         <v>568</v>
       </c>
@@ -29162,10 +29162,10 @@
         <f t="shared" si="8"/>
         <v>116</v>
       </c>
-      <c r="M176" s="200" t="s">
+      <c r="M176" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="N176" s="201"/>
+      <c r="N176" s="163"/>
       <c r="O176" s="2" t="s">
         <v>568</v>
       </c>
@@ -29472,10 +29472,10 @@
         <f t="shared" si="8"/>
         <v>82</v>
       </c>
-      <c r="M180" s="250" t="s">
+      <c r="M180" s="246" t="s">
         <v>18</v>
       </c>
-      <c r="N180" s="251"/>
+      <c r="N180" s="247"/>
       <c r="O180" s="2" t="s">
         <v>427</v>
       </c>
@@ -29545,10 +29545,10 @@
         <f t="shared" si="8"/>
         <v>112</v>
       </c>
-      <c r="M181" s="252" t="s">
+      <c r="M181" s="248" t="s">
         <v>18</v>
       </c>
-      <c r="N181" s="253"/>
+      <c r="N181" s="249"/>
       <c r="O181" s="2" t="s">
         <v>427</v>
       </c>
@@ -29618,10 +29618,10 @@
         <f t="shared" si="8"/>
         <v>172</v>
       </c>
-      <c r="M182" s="254" t="s">
+      <c r="M182" s="250" t="s">
         <v>18</v>
       </c>
-      <c r="N182" s="255"/>
+      <c r="N182" s="251"/>
       <c r="O182" s="2" t="s">
         <v>427</v>
       </c>
@@ -29691,10 +29691,10 @@
         <f t="shared" si="8"/>
         <v>189</v>
       </c>
-      <c r="M183" s="256" t="s">
+      <c r="M183" s="252" t="s">
         <v>11</v>
       </c>
-      <c r="N183" s="257"/>
+      <c r="N183" s="253"/>
       <c r="O183" s="2" t="s">
         <v>443</v>
       </c>
@@ -29764,10 +29764,10 @@
         <f t="shared" si="8"/>
         <v>93</v>
       </c>
-      <c r="M184" s="202" t="s">
+      <c r="M184" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N184" s="203"/>
+      <c r="N184" s="183"/>
       <c r="O184" s="2" t="s">
         <v>569</v>
       </c>
@@ -29837,10 +29837,10 @@
         <f t="shared" si="8"/>
         <v>152</v>
       </c>
-      <c r="M185" s="202" t="s">
+      <c r="M185" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N185" s="203"/>
+      <c r="N185" s="183"/>
       <c r="O185" s="2" t="s">
         <v>569</v>
       </c>
@@ -29910,10 +29910,10 @@
         <f t="shared" si="8"/>
         <v>198</v>
       </c>
-      <c r="M186" s="244" t="s">
+      <c r="M186" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="N186" s="245"/>
+      <c r="N186" s="265"/>
       <c r="O186" s="2" t="s">
         <v>454</v>
       </c>
@@ -29983,10 +29983,10 @@
         <f t="shared" si="8"/>
         <v>192</v>
       </c>
-      <c r="M187" s="202" t="s">
+      <c r="M187" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N187" s="203"/>
+      <c r="N187" s="183"/>
       <c r="O187" s="2" t="s">
         <v>420</v>
       </c>
@@ -30287,10 +30287,10 @@
         <f t="shared" si="8"/>
         <v>112</v>
       </c>
-      <c r="M191" s="200" t="s">
+      <c r="M191" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N191" s="201"/>
+      <c r="N191" s="163"/>
       <c r="O191" s="2" t="s">
         <v>425</v>
       </c>
@@ -30360,10 +30360,10 @@
         <f t="shared" si="8"/>
         <v>55</v>
       </c>
-      <c r="M192" s="246" t="s">
+      <c r="M192" s="242" t="s">
         <v>11</v>
       </c>
-      <c r="N192" s="247"/>
+      <c r="N192" s="243"/>
       <c r="O192" s="2" t="s">
         <v>443</v>
       </c>
@@ -30433,10 +30433,10 @@
         <f t="shared" si="8"/>
         <v>148</v>
       </c>
-      <c r="M193" s="204" t="s">
+      <c r="M193" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="N193" s="205"/>
+      <c r="N193" s="271"/>
       <c r="O193" s="2" t="s">
         <v>443</v>
       </c>
@@ -30731,10 +30731,10 @@
         <f t="shared" si="11"/>
         <v>194</v>
       </c>
-      <c r="M197" s="248" t="s">
+      <c r="M197" s="244" t="s">
         <v>21</v>
       </c>
-      <c r="N197" s="249"/>
+      <c r="N197" s="245"/>
       <c r="O197" s="2" t="s">
         <v>434</v>
       </c>
@@ -30804,10 +30804,10 @@
         <f t="shared" si="11"/>
         <v>250</v>
       </c>
-      <c r="M198" s="206" t="s">
+      <c r="M198" s="272" t="s">
         <v>27</v>
       </c>
-      <c r="N198" s="207"/>
+      <c r="N198" s="273"/>
       <c r="O198" s="2" t="s">
         <v>457</v>
       </c>
@@ -31027,10 +31027,10 @@
         <f t="shared" si="11"/>
         <v>167</v>
       </c>
-      <c r="M201" s="218" t="s">
+      <c r="M201" s="278" t="s">
         <v>25</v>
       </c>
-      <c r="N201" s="219"/>
+      <c r="N201" s="279"/>
       <c r="O201" s="2" t="s">
         <v>459</v>
       </c>
@@ -31100,10 +31100,10 @@
         <f t="shared" si="11"/>
         <v>91</v>
       </c>
-      <c r="M202" s="220" t="s">
+      <c r="M202" s="280" t="s">
         <v>21</v>
       </c>
-      <c r="N202" s="221"/>
+      <c r="N202" s="281"/>
       <c r="O202" s="2" t="s">
         <v>434</v>
       </c>
@@ -31173,10 +31173,10 @@
         <f t="shared" si="11"/>
         <v>106</v>
       </c>
-      <c r="M203" s="222" t="s">
+      <c r="M203" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="N203" s="223"/>
+      <c r="N203" s="193"/>
       <c r="O203" s="2" t="s">
         <v>434</v>
       </c>
@@ -31321,10 +31321,10 @@
         <f t="shared" si="11"/>
         <v>146</v>
       </c>
-      <c r="M205" s="224" t="s">
+      <c r="M205" s="282" t="s">
         <v>16</v>
       </c>
-      <c r="N205" s="225"/>
+      <c r="N205" s="283"/>
       <c r="O205" s="2" t="s">
         <v>421</v>
       </c>
@@ -31469,10 +31469,10 @@
         <f t="shared" si="11"/>
         <v>131</v>
       </c>
-      <c r="M207" s="210" t="s">
+      <c r="M207" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N207" s="211"/>
+      <c r="N207" s="173"/>
       <c r="O207" s="2" t="s">
         <v>425</v>
       </c>
@@ -31692,10 +31692,10 @@
         <f t="shared" si="11"/>
         <v>89</v>
       </c>
-      <c r="M210" s="200" t="s">
+      <c r="M210" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="N210" s="201"/>
+      <c r="N210" s="163"/>
       <c r="O210" s="2" t="s">
         <v>568</v>
       </c>
@@ -31765,10 +31765,10 @@
         <f t="shared" si="11"/>
         <v>137</v>
       </c>
-      <c r="M211" s="214" t="s">
+      <c r="M211" s="276" t="s">
         <v>30</v>
       </c>
-      <c r="N211" s="215"/>
+      <c r="N211" s="277"/>
       <c r="O211" s="2" t="s">
         <v>568</v>
       </c>
@@ -32213,10 +32213,10 @@
         <f t="shared" si="11"/>
         <v>93</v>
       </c>
-      <c r="M217" s="210" t="s">
+      <c r="M217" s="172" t="s">
         <v>17</v>
       </c>
-      <c r="N217" s="211"/>
+      <c r="N217" s="173"/>
       <c r="O217" s="2" t="s">
         <v>425</v>
       </c>
@@ -32286,10 +32286,10 @@
         <f t="shared" si="11"/>
         <v>144</v>
       </c>
-      <c r="M218" s="212" t="s">
+      <c r="M218" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="N218" s="213"/>
+      <c r="N218" s="175"/>
       <c r="O218" s="2" t="s">
         <v>425</v>
       </c>
@@ -32359,10 +32359,10 @@
         <f t="shared" si="11"/>
         <v>71</v>
       </c>
-      <c r="M219" s="216" t="s">
+      <c r="M219" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N219" s="217"/>
+      <c r="N219" s="177"/>
       <c r="O219" s="2" t="s">
         <v>418</v>
       </c>
@@ -32732,10 +32732,10 @@
         <f t="shared" si="11"/>
         <v>69</v>
       </c>
-      <c r="M224" s="202" t="s">
+      <c r="M224" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N224" s="203"/>
+      <c r="N224" s="183"/>
       <c r="O224" s="2" t="s">
         <v>420</v>
       </c>
@@ -32805,10 +32805,10 @@
         <f t="shared" si="11"/>
         <v>141</v>
       </c>
-      <c r="M225" s="202" t="s">
+      <c r="M225" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N225" s="203"/>
+      <c r="N225" s="183"/>
       <c r="O225" s="2" t="s">
         <v>420</v>
       </c>
@@ -33340,10 +33340,10 @@
         <f t="shared" si="11"/>
         <v>107</v>
       </c>
-      <c r="M232" s="240" t="s">
+      <c r="M232" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="N232" s="241"/>
+      <c r="N232" s="167"/>
       <c r="O232" s="2" t="s">
         <v>428</v>
       </c>
@@ -33413,10 +33413,10 @@
         <f t="shared" si="11"/>
         <v>214</v>
       </c>
-      <c r="M233" s="242" t="s">
+      <c r="M233" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="N233" s="243"/>
+      <c r="N233" s="169"/>
       <c r="O233" s="2" t="s">
         <v>428</v>
       </c>
@@ -33486,10 +33486,10 @@
         <f t="shared" si="11"/>
         <v>183</v>
       </c>
-      <c r="M234" s="200" t="s">
+      <c r="M234" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N234" s="201"/>
+      <c r="N234" s="163"/>
       <c r="O234" s="2" t="s">
         <v>425</v>
       </c>
@@ -33559,10 +33559,10 @@
         <f t="shared" si="11"/>
         <v>132</v>
       </c>
-      <c r="M235" s="200" t="s">
+      <c r="M235" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N235" s="201"/>
+      <c r="N235" s="163"/>
       <c r="O235" s="2" t="s">
         <v>425</v>
       </c>
@@ -33632,10 +33632,10 @@
         <f t="shared" si="11"/>
         <v>88</v>
       </c>
-      <c r="M236" s="208" t="s">
+      <c r="M236" s="274" t="s">
         <v>17</v>
       </c>
-      <c r="N236" s="209"/>
+      <c r="N236" s="275"/>
       <c r="O236" s="2" t="s">
         <v>425</v>
       </c>
@@ -33705,10 +33705,10 @@
         <f t="shared" si="11"/>
         <v>64</v>
       </c>
-      <c r="M237" s="192" t="s">
+      <c r="M237" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N237" s="193"/>
+      <c r="N237" s="207"/>
       <c r="O237" s="2" t="s">
         <v>432</v>
       </c>
@@ -33778,10 +33778,10 @@
         <f t="shared" si="11"/>
         <v>214</v>
       </c>
-      <c r="M238" s="192" t="s">
+      <c r="M238" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="N238" s="193"/>
+      <c r="N238" s="207"/>
       <c r="O238" s="2" t="s">
         <v>432</v>
       </c>
@@ -33932,10 +33932,10 @@
         <f t="shared" si="11"/>
         <v>110</v>
       </c>
-      <c r="M240" s="236" t="s">
+      <c r="M240" s="224" t="s">
         <v>18</v>
       </c>
-      <c r="N240" s="237"/>
+      <c r="N240" s="225"/>
       <c r="O240" s="2" t="s">
         <v>427</v>
       </c>
@@ -34011,10 +34011,10 @@
         <f t="shared" si="11"/>
         <v>108</v>
       </c>
-      <c r="M241" s="216" t="s">
+      <c r="M241" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N241" s="217"/>
+      <c r="N241" s="177"/>
       <c r="O241" s="2" t="s">
         <v>418</v>
       </c>
@@ -34084,10 +34084,10 @@
         <f t="shared" si="11"/>
         <v>211</v>
       </c>
-      <c r="M242" s="238" t="s">
+      <c r="M242" s="262" t="s">
         <v>17</v>
       </c>
-      <c r="N242" s="239"/>
+      <c r="N242" s="263"/>
       <c r="O242" s="2" t="s">
         <v>425</v>
       </c>
@@ -34157,10 +34157,10 @@
         <f t="shared" si="11"/>
         <v>229</v>
       </c>
-      <c r="M243" s="200" t="s">
+      <c r="M243" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="N243" s="201"/>
+      <c r="N243" s="163"/>
       <c r="O243" s="2" t="s">
         <v>425</v>
       </c>
@@ -34230,10 +34230,10 @@
         <f t="shared" si="11"/>
         <v>210</v>
       </c>
-      <c r="M244" s="232" t="s">
+      <c r="M244" s="258" t="s">
         <v>18</v>
       </c>
-      <c r="N244" s="233"/>
+      <c r="N244" s="259"/>
       <c r="O244" s="2" t="s">
         <v>427</v>
       </c>
@@ -34303,10 +34303,10 @@
         <f t="shared" si="11"/>
         <v>176</v>
       </c>
-      <c r="M245" s="216" t="s">
+      <c r="M245" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="N245" s="217"/>
+      <c r="N245" s="177"/>
       <c r="O245" s="2" t="s">
         <v>418</v>
       </c>
@@ -34376,10 +34376,10 @@
         <f t="shared" si="11"/>
         <v>235</v>
       </c>
-      <c r="M246" s="194" t="s">
+      <c r="M246" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="N246" s="195"/>
+      <c r="N246" s="213"/>
       <c r="O246" s="2" t="s">
         <v>420</v>
       </c>
@@ -34902,10 +34902,10 @@
         <f t="shared" si="11"/>
         <v>104</v>
       </c>
-      <c r="M253" s="196" t="s">
+      <c r="M253" s="266" t="s">
         <v>11</v>
       </c>
-      <c r="N253" s="197"/>
+      <c r="N253" s="267"/>
       <c r="O253" s="2" t="s">
         <v>443</v>
       </c>
@@ -34975,10 +34975,10 @@
         <f t="shared" si="11"/>
         <v>130</v>
       </c>
-      <c r="M254" s="180" t="s">
+      <c r="M254" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N254" s="181"/>
+      <c r="N254" s="269"/>
       <c r="O254" s="2" t="s">
         <v>443</v>
       </c>
@@ -35048,10 +35048,10 @@
         <f t="shared" si="11"/>
         <v>180</v>
       </c>
-      <c r="M255" s="180" t="s">
+      <c r="M255" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N255" s="181"/>
+      <c r="N255" s="269"/>
       <c r="O255" s="2" t="s">
         <v>443</v>
       </c>
@@ -35121,10 +35121,10 @@
         <f t="shared" si="11"/>
         <v>92</v>
       </c>
-      <c r="M256" s="184" t="s">
+      <c r="M256" s="288" t="s">
         <v>13</v>
       </c>
-      <c r="N256" s="185"/>
+      <c r="N256" s="289"/>
       <c r="O256" s="2" t="s">
         <v>418</v>
       </c>
@@ -35350,10 +35350,10 @@
         <f t="shared" ref="L259:L322" si="14">ROUND((1+(H259-75)/500)*(ROUND(0.25*(7*MAX(G259,E259)+MIN(G259,E259)),0)),0)</f>
         <v>93</v>
       </c>
-      <c r="M259" s="160" t="s">
+      <c r="M259" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N259" s="161"/>
+      <c r="N259" s="291"/>
       <c r="O259" s="2" t="s">
         <v>420</v>
       </c>
@@ -35573,10 +35573,10 @@
         <f t="shared" si="14"/>
         <v>63</v>
       </c>
-      <c r="M262" s="176" t="s">
+      <c r="M262" s="292" t="s">
         <v>27</v>
       </c>
-      <c r="N262" s="177"/>
+      <c r="N262" s="293"/>
       <c r="O262" s="2" t="s">
         <v>457</v>
       </c>
@@ -35646,10 +35646,10 @@
         <f t="shared" si="14"/>
         <v>137</v>
       </c>
-      <c r="M263" s="176" t="s">
+      <c r="M263" s="292" t="s">
         <v>27</v>
       </c>
-      <c r="N263" s="177"/>
+      <c r="N263" s="293"/>
       <c r="O263" s="2" t="s">
         <v>457</v>
       </c>
@@ -35719,10 +35719,10 @@
         <f t="shared" si="14"/>
         <v>80</v>
       </c>
-      <c r="M264" s="178" t="s">
+      <c r="M264" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N264" s="179"/>
+      <c r="N264" s="287"/>
       <c r="O264" s="2" t="s">
         <v>425</v>
       </c>
@@ -35792,10 +35792,10 @@
         <f t="shared" si="14"/>
         <v>128</v>
       </c>
-      <c r="M265" s="178" t="s">
+      <c r="M265" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N265" s="179"/>
+      <c r="N265" s="287"/>
       <c r="O265" s="2" t="s">
         <v>425</v>
       </c>
@@ -35865,10 +35865,10 @@
         <f t="shared" si="14"/>
         <v>61</v>
       </c>
-      <c r="M266" s="188" t="s">
+      <c r="M266" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="N266" s="189"/>
+      <c r="N266" s="285"/>
       <c r="O266" s="2" t="s">
         <v>421</v>
       </c>
@@ -35938,10 +35938,10 @@
         <f t="shared" si="14"/>
         <v>91</v>
       </c>
-      <c r="M267" s="188" t="s">
+      <c r="M267" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="N267" s="189"/>
+      <c r="N267" s="285"/>
       <c r="O267" s="2" t="s">
         <v>421</v>
       </c>
@@ -36086,10 +36086,10 @@
         <f t="shared" si="14"/>
         <v>91</v>
       </c>
-      <c r="M269" s="188" t="s">
+      <c r="M269" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="N269" s="189"/>
+      <c r="N269" s="285"/>
       <c r="O269" s="2" t="s">
         <v>421</v>
       </c>
@@ -36459,10 +36459,10 @@
         <f t="shared" si="14"/>
         <v>86</v>
       </c>
-      <c r="M274" s="180" t="s">
+      <c r="M274" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N274" s="181"/>
+      <c r="N274" s="269"/>
       <c r="O274" s="2" t="s">
         <v>443</v>
       </c>
@@ -37357,10 +37357,10 @@
         <f t="shared" si="14"/>
         <v>110</v>
       </c>
-      <c r="M286" s="180" t="s">
+      <c r="M286" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N286" s="181"/>
+      <c r="N286" s="269"/>
       <c r="O286" s="2" t="s">
         <v>443</v>
       </c>
@@ -37505,10 +37505,10 @@
         <f t="shared" si="14"/>
         <v>104</v>
       </c>
-      <c r="M288" s="178" t="s">
+      <c r="M288" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N288" s="179"/>
+      <c r="N288" s="287"/>
       <c r="O288" s="2" t="s">
         <v>425</v>
       </c>
@@ -37578,10 +37578,10 @@
         <f t="shared" si="14"/>
         <v>159</v>
       </c>
-      <c r="M289" s="178" t="s">
+      <c r="M289" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N289" s="179"/>
+      <c r="N289" s="287"/>
       <c r="O289" s="2" t="s">
         <v>425</v>
       </c>
@@ -37648,10 +37648,10 @@
       <c r="L290" s="2">
         <v>183</v>
       </c>
-      <c r="M290" s="178" t="s">
+      <c r="M290" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N290" s="179"/>
+      <c r="N290" s="287"/>
       <c r="O290" s="2" t="s">
         <v>425</v>
       </c>
@@ -37946,10 +37946,10 @@
         <f t="shared" si="14"/>
         <v>42</v>
       </c>
-      <c r="M294" s="178" t="s">
+      <c r="M294" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N294" s="179"/>
+      <c r="N294" s="287"/>
       <c r="O294" s="2" t="s">
         <v>425</v>
       </c>
@@ -38019,10 +38019,10 @@
         <f t="shared" si="14"/>
         <v>81</v>
       </c>
-      <c r="M295" s="178" t="s">
+      <c r="M295" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N295" s="179"/>
+      <c r="N295" s="287"/>
       <c r="O295" s="2" t="s">
         <v>425</v>
       </c>
@@ -38092,10 +38092,10 @@
         <f t="shared" si="14"/>
         <v>142</v>
       </c>
-      <c r="M296" s="178" t="s">
+      <c r="M296" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N296" s="179"/>
+      <c r="N296" s="287"/>
       <c r="O296" s="2" t="s">
         <v>425</v>
       </c>
@@ -38165,10 +38165,10 @@
         <f t="shared" si="14"/>
         <v>54</v>
       </c>
-      <c r="M297" s="190" t="s">
+      <c r="M297" s="294" t="s">
         <v>20</v>
       </c>
-      <c r="N297" s="191"/>
+      <c r="N297" s="295"/>
       <c r="O297" s="2" t="s">
         <v>432</v>
       </c>
@@ -38238,10 +38238,10 @@
         <f t="shared" si="14"/>
         <v>114</v>
       </c>
-      <c r="M298" s="190" t="s">
+      <c r="M298" s="294" t="s">
         <v>20</v>
       </c>
-      <c r="N298" s="191"/>
+      <c r="N298" s="295"/>
       <c r="O298" s="2" t="s">
         <v>432</v>
       </c>
@@ -38386,10 +38386,10 @@
         <f t="shared" si="14"/>
         <v>236</v>
       </c>
-      <c r="M300" s="168" t="s">
+      <c r="M300" s="296" t="s">
         <v>22</v>
       </c>
-      <c r="N300" s="169"/>
+      <c r="N300" s="297"/>
       <c r="O300" s="2" t="s">
         <v>454</v>
       </c>
@@ -38459,10 +38459,10 @@
         <f t="shared" si="14"/>
         <v>84</v>
       </c>
-      <c r="M301" s="178" t="s">
+      <c r="M301" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N301" s="179"/>
+      <c r="N301" s="287"/>
       <c r="O301" s="2" t="s">
         <v>425</v>
       </c>
@@ -38532,10 +38532,10 @@
         <f t="shared" si="14"/>
         <v>132</v>
       </c>
-      <c r="M302" s="178" t="s">
+      <c r="M302" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N302" s="179"/>
+      <c r="N302" s="287"/>
       <c r="O302" s="2" t="s">
         <v>425</v>
       </c>
@@ -39130,10 +39130,10 @@
         <f t="shared" si="14"/>
         <v>78</v>
       </c>
-      <c r="M310" s="186" t="s">
+      <c r="M310" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="N310" s="187"/>
+      <c r="N310" s="299"/>
       <c r="O310" s="2" t="s">
         <v>427</v>
       </c>
@@ -39203,10 +39203,10 @@
         <f t="shared" si="14"/>
         <v>127</v>
       </c>
-      <c r="M311" s="186" t="s">
+      <c r="M311" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="N311" s="187"/>
+      <c r="N311" s="299"/>
       <c r="O311" s="2" t="s">
         <v>427</v>
       </c>
@@ -39276,10 +39276,10 @@
         <f t="shared" si="14"/>
         <v>147</v>
       </c>
-      <c r="M312" s="186" t="s">
+      <c r="M312" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="N312" s="187"/>
+      <c r="N312" s="299"/>
       <c r="O312" s="2" t="s">
         <v>427</v>
       </c>
@@ -39349,10 +39349,10 @@
         <f t="shared" si="14"/>
         <v>167</v>
       </c>
-      <c r="M313" s="186" t="s">
+      <c r="M313" s="298" t="s">
         <v>18</v>
       </c>
-      <c r="N313" s="187"/>
+      <c r="N313" s="299"/>
       <c r="O313" s="2" t="s">
         <v>427</v>
       </c>
@@ -39422,10 +39422,10 @@
         <f t="shared" si="14"/>
         <v>171</v>
       </c>
-      <c r="M314" s="188" t="s">
+      <c r="M314" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="N314" s="189"/>
+      <c r="N314" s="285"/>
       <c r="O314" s="2" t="s">
         <v>421</v>
       </c>
@@ -39495,10 +39495,10 @@
         <f t="shared" si="14"/>
         <v>171</v>
       </c>
-      <c r="M315" s="188" t="s">
+      <c r="M315" s="284" t="s">
         <v>16</v>
       </c>
-      <c r="N315" s="189"/>
+      <c r="N315" s="285"/>
       <c r="O315" s="2" t="s">
         <v>421</v>
       </c>
@@ -39643,10 +39643,10 @@
         <f t="shared" si="14"/>
         <v>99</v>
       </c>
-      <c r="M317" s="182" t="s">
+      <c r="M317" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="N317" s="183"/>
+      <c r="N317" s="303"/>
       <c r="O317" s="2" t="s">
         <v>426</v>
       </c>
@@ -39716,10 +39716,10 @@
         <f t="shared" si="14"/>
         <v>159</v>
       </c>
-      <c r="M318" s="182" t="s">
+      <c r="M318" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="N318" s="183"/>
+      <c r="N318" s="303"/>
       <c r="O318" s="2" t="s">
         <v>426</v>
       </c>
@@ -39939,10 +39939,10 @@
         <f t="shared" si="14"/>
         <v>68</v>
       </c>
-      <c r="M321" s="160" t="s">
+      <c r="M321" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N321" s="161"/>
+      <c r="N321" s="291"/>
       <c r="O321" s="2" t="s">
         <v>420</v>
       </c>
@@ -40012,10 +40012,10 @@
         <f t="shared" si="14"/>
         <v>87</v>
       </c>
-      <c r="M322" s="160" t="s">
+      <c r="M322" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N322" s="161"/>
+      <c r="N322" s="291"/>
       <c r="O322" s="2" t="s">
         <v>420</v>
       </c>
@@ -40235,10 +40235,10 @@
         <f t="shared" si="17"/>
         <v>234</v>
       </c>
-      <c r="M325" s="184" t="s">
+      <c r="M325" s="288" t="s">
         <v>13</v>
       </c>
-      <c r="N325" s="185"/>
+      <c r="N325" s="289"/>
       <c r="O325" s="2" t="s">
         <v>418</v>
       </c>
@@ -40308,10 +40308,10 @@
         <f t="shared" si="17"/>
         <v>145</v>
       </c>
-      <c r="M326" s="164" t="s">
+      <c r="M326" s="300" t="s">
         <v>21</v>
       </c>
-      <c r="N326" s="165"/>
+      <c r="N326" s="301"/>
       <c r="O326" s="2" t="s">
         <v>434</v>
       </c>
@@ -40381,10 +40381,10 @@
         <f t="shared" si="17"/>
         <v>211</v>
       </c>
-      <c r="M327" s="164" t="s">
+      <c r="M327" s="300" t="s">
         <v>21</v>
       </c>
-      <c r="N327" s="165"/>
+      <c r="N327" s="301"/>
       <c r="O327" s="2" t="s">
         <v>434</v>
       </c>
@@ -40454,10 +40454,10 @@
         <f t="shared" si="17"/>
         <v>116</v>
       </c>
-      <c r="M328" s="178" t="s">
+      <c r="M328" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N328" s="179"/>
+      <c r="N328" s="287"/>
       <c r="O328" s="2" t="s">
         <v>425</v>
       </c>
@@ -40527,10 +40527,10 @@
         <f t="shared" si="17"/>
         <v>78</v>
       </c>
-      <c r="M329" s="162" t="s">
+      <c r="M329" s="304" t="s">
         <v>19</v>
       </c>
-      <c r="N329" s="163"/>
+      <c r="N329" s="305"/>
       <c r="O329" s="2" t="s">
         <v>428</v>
       </c>
@@ -40750,10 +40750,10 @@
         <f t="shared" si="17"/>
         <v>74</v>
       </c>
-      <c r="M332" s="180" t="s">
+      <c r="M332" s="268" t="s">
         <v>11</v>
       </c>
-      <c r="N332" s="181"/>
+      <c r="N332" s="269"/>
       <c r="O332" s="2" t="s">
         <v>443</v>
       </c>
@@ -41048,10 +41048,10 @@
         <f t="shared" si="17"/>
         <v>124</v>
       </c>
-      <c r="M336" s="178" t="s">
+      <c r="M336" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N336" s="179"/>
+      <c r="N336" s="287"/>
       <c r="O336" s="2" t="s">
         <v>425</v>
       </c>
@@ -41121,10 +41121,10 @@
         <f t="shared" si="17"/>
         <v>118</v>
       </c>
-      <c r="M337" s="182" t="s">
+      <c r="M337" s="302" t="s">
         <v>12</v>
       </c>
-      <c r="N337" s="183"/>
+      <c r="N337" s="303"/>
       <c r="O337" s="2" t="s">
         <v>426</v>
       </c>
@@ -41494,10 +41494,10 @@
         <f t="shared" si="17"/>
         <v>113</v>
       </c>
-      <c r="M342" s="160" t="s">
+      <c r="M342" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N342" s="161"/>
+      <c r="N342" s="291"/>
       <c r="O342" s="2" t="s">
         <v>420</v>
       </c>
@@ -42092,10 +42092,10 @@
         <f t="shared" si="17"/>
         <v>102</v>
       </c>
-      <c r="M350" s="160" t="s">
+      <c r="M350" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N350" s="161"/>
+      <c r="N350" s="291"/>
       <c r="O350" s="2" t="s">
         <v>420</v>
       </c>
@@ -42165,10 +42165,10 @@
         <f t="shared" si="17"/>
         <v>242</v>
       </c>
-      <c r="M351" s="160" t="s">
+      <c r="M351" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N351" s="161"/>
+      <c r="N351" s="291"/>
       <c r="O351" s="2" t="s">
         <v>420</v>
       </c>
@@ -42244,10 +42244,10 @@
         <f t="shared" si="17"/>
         <v>139</v>
       </c>
-      <c r="M352" s="178" t="s">
+      <c r="M352" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N352" s="179"/>
+      <c r="N352" s="287"/>
       <c r="O352" s="2" t="s">
         <v>425</v>
       </c>
@@ -42317,10 +42317,10 @@
         <f t="shared" si="17"/>
         <v>212</v>
       </c>
-      <c r="M353" s="178" t="s">
+      <c r="M353" s="286" t="s">
         <v>17</v>
       </c>
-      <c r="N353" s="179"/>
+      <c r="N353" s="287"/>
       <c r="O353" s="2" t="s">
         <v>425</v>
       </c>
@@ -42390,10 +42390,10 @@
         <f t="shared" si="17"/>
         <v>66</v>
       </c>
-      <c r="M354" s="174" t="s">
+      <c r="M354" s="308" t="s">
         <v>25</v>
       </c>
-      <c r="N354" s="175"/>
+      <c r="N354" s="309"/>
       <c r="O354" s="2" t="s">
         <v>459</v>
       </c>
@@ -42463,10 +42463,10 @@
         <f t="shared" si="17"/>
         <v>127</v>
       </c>
-      <c r="M355" s="174" t="s">
+      <c r="M355" s="308" t="s">
         <v>25</v>
       </c>
-      <c r="N355" s="175"/>
+      <c r="N355" s="309"/>
       <c r="O355" s="2" t="s">
         <v>459</v>
       </c>
@@ -42536,10 +42536,10 @@
         <f t="shared" si="17"/>
         <v>162</v>
       </c>
-      <c r="M356" s="174" t="s">
+      <c r="M356" s="308" t="s">
         <v>25</v>
       </c>
-      <c r="N356" s="175"/>
+      <c r="N356" s="309"/>
       <c r="O356" s="2" t="s">
         <v>459</v>
       </c>
@@ -42609,10 +42609,10 @@
         <f t="shared" si="17"/>
         <v>234</v>
       </c>
-      <c r="M357" s="174" t="s">
+      <c r="M357" s="308" t="s">
         <v>25</v>
       </c>
-      <c r="N357" s="175"/>
+      <c r="N357" s="309"/>
       <c r="O357" s="2" t="s">
         <v>459</v>
       </c>
@@ -42757,10 +42757,10 @@
         <f t="shared" si="17"/>
         <v>174</v>
       </c>
-      <c r="M359" s="164" t="s">
+      <c r="M359" s="300" t="s">
         <v>21</v>
       </c>
-      <c r="N359" s="165"/>
+      <c r="N359" s="301"/>
       <c r="O359" s="2" t="s">
         <v>434</v>
       </c>
@@ -42830,10 +42830,10 @@
         <f t="shared" si="17"/>
         <v>120</v>
       </c>
-      <c r="M360" s="176" t="s">
+      <c r="M360" s="292" t="s">
         <v>27</v>
       </c>
-      <c r="N360" s="177"/>
+      <c r="N360" s="293"/>
       <c r="O360" s="2" t="s">
         <v>457</v>
       </c>
@@ -42903,10 +42903,10 @@
         <f t="shared" si="17"/>
         <v>86</v>
       </c>
-      <c r="M361" s="164" t="s">
+      <c r="M361" s="300" t="s">
         <v>21</v>
       </c>
-      <c r="N361" s="165"/>
+      <c r="N361" s="301"/>
       <c r="O361" s="2" t="s">
         <v>434</v>
       </c>
@@ -42976,10 +42976,10 @@
         <f t="shared" si="17"/>
         <v>95</v>
       </c>
-      <c r="M362" s="170" t="s">
+      <c r="M362" s="306" t="s">
         <v>24</v>
       </c>
-      <c r="N362" s="171"/>
+      <c r="N362" s="307"/>
       <c r="O362" s="2" t="s">
         <v>495</v>
       </c>
@@ -43049,10 +43049,10 @@
         <f t="shared" si="17"/>
         <v>162</v>
       </c>
-      <c r="M363" s="170" t="s">
+      <c r="M363" s="306" t="s">
         <v>24</v>
       </c>
-      <c r="N363" s="171"/>
+      <c r="N363" s="307"/>
       <c r="O363" s="2" t="s">
         <v>495</v>
       </c>
@@ -43347,10 +43347,10 @@
         <f t="shared" si="17"/>
         <v>149</v>
       </c>
-      <c r="M367" s="160" t="s">
+      <c r="M367" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N367" s="161"/>
+      <c r="N367" s="291"/>
       <c r="O367" s="2" t="s">
         <v>420</v>
       </c>
@@ -43420,10 +43420,10 @@
         <f t="shared" si="17"/>
         <v>194</v>
       </c>
-      <c r="M368" s="160" t="s">
+      <c r="M368" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N368" s="161"/>
+      <c r="N368" s="291"/>
       <c r="O368" s="2" t="s">
         <v>420</v>
       </c>
@@ -43493,10 +43493,10 @@
         <f t="shared" si="17"/>
         <v>194</v>
       </c>
-      <c r="M369" s="160" t="s">
+      <c r="M369" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N369" s="161"/>
+      <c r="N369" s="291"/>
       <c r="O369" s="2" t="s">
         <v>420</v>
       </c>
@@ -43641,10 +43641,10 @@
         <f t="shared" si="17"/>
         <v>134</v>
       </c>
-      <c r="M371" s="160" t="s">
+      <c r="M371" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N371" s="161"/>
+      <c r="N371" s="291"/>
       <c r="O371" s="2" t="s">
         <v>420</v>
       </c>
@@ -43714,10 +43714,10 @@
         <f t="shared" si="17"/>
         <v>107</v>
       </c>
-      <c r="M372" s="166" t="s">
+      <c r="M372" s="310" t="s">
         <v>26</v>
       </c>
-      <c r="N372" s="167"/>
+      <c r="N372" s="311"/>
       <c r="O372" s="2" t="s">
         <v>450</v>
       </c>
@@ -43787,10 +43787,10 @@
         <f t="shared" si="17"/>
         <v>179</v>
       </c>
-      <c r="M373" s="166" t="s">
+      <c r="M373" s="310" t="s">
         <v>26</v>
       </c>
-      <c r="N373" s="167"/>
+      <c r="N373" s="311"/>
       <c r="O373" s="2" t="s">
         <v>450</v>
       </c>
@@ -44082,8 +44082,7 @@
         <v>257</v>
       </c>
       <c r="L377" s="2">
-        <f t="shared" si="17"/>
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M377" s="82" t="s">
         <v>23</v>
@@ -44160,10 +44159,10 @@
         <f t="shared" si="17"/>
         <v>356</v>
       </c>
-      <c r="M378" s="168" t="s">
+      <c r="M378" s="296" t="s">
         <v>22</v>
       </c>
-      <c r="N378" s="169"/>
+      <c r="N378" s="297"/>
       <c r="O378" s="2" t="s">
         <v>454</v>
       </c>
@@ -44233,10 +44232,10 @@
         <f t="shared" si="17"/>
         <v>356</v>
       </c>
-      <c r="M379" s="170" t="s">
+      <c r="M379" s="306" t="s">
         <v>24</v>
       </c>
-      <c r="N379" s="171"/>
+      <c r="N379" s="307"/>
       <c r="O379" s="2" t="s">
         <v>495</v>
       </c>
@@ -44306,10 +44305,10 @@
         <f t="shared" si="17"/>
         <v>285</v>
       </c>
-      <c r="M380" s="172" t="s">
+      <c r="M380" s="312" t="s">
         <v>23</v>
       </c>
-      <c r="N380" s="173"/>
+      <c r="N380" s="313"/>
       <c r="O380" s="2" t="s">
         <v>498</v>
       </c>
@@ -44526,10 +44525,10 @@
       <c r="L383" s="2">
         <v>251</v>
       </c>
-      <c r="M383" s="160" t="s">
+      <c r="M383" s="290" t="s">
         <v>15</v>
       </c>
-      <c r="N383" s="161"/>
+      <c r="N383" s="291"/>
       <c r="O383" s="2" t="s">
         <v>420</v>
       </c>
@@ -44602,10 +44601,10 @@
       <c r="L384" s="2">
         <v>251</v>
       </c>
-      <c r="M384" s="162" t="s">
+      <c r="M384" s="304" t="s">
         <v>19</v>
       </c>
-      <c r="N384" s="163"/>
+      <c r="N384" s="305"/>
       <c r="O384" s="2" t="s">
         <v>428</v>
       </c>
@@ -44822,10 +44821,10 @@
         <f t="shared" ref="L387:L445" si="19">ROUND((1+(H387-75)/500)*(ROUND(0.25*(7*MAX(G387,E387)+MIN(G387,E387)),0)),0)</f>
         <v>115</v>
       </c>
-      <c r="M387" s="164" t="s">
+      <c r="M387" s="300" t="s">
         <v>21</v>
       </c>
-      <c r="N387" s="165"/>
+      <c r="N387" s="301"/>
       <c r="O387" s="2" t="s">
         <v>434</v>
       </c>
@@ -70741,99 +70740,95 @@
     </row>
   </sheetData>
   <mergeCells count="206">
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="M98:N98"/>
-    <mergeCell ref="M99:N99"/>
-    <mergeCell ref="M100:N100"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="M78:N78"/>
-    <mergeCell ref="M89:N89"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="M79:N79"/>
-    <mergeCell ref="M87:N87"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M65:N65"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="M67:N67"/>
-    <mergeCell ref="M68:N68"/>
-    <mergeCell ref="M56:N56"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="M58:N58"/>
-    <mergeCell ref="M59:N59"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="M110:N110"/>
-    <mergeCell ref="M114:N114"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="M109:N109"/>
-    <mergeCell ref="M127:N127"/>
-    <mergeCell ref="M128:N128"/>
-    <mergeCell ref="M129:N129"/>
-    <mergeCell ref="M133:N133"/>
-    <mergeCell ref="M134:N134"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="M119:N119"/>
-    <mergeCell ref="M120:N120"/>
-    <mergeCell ref="M126:N126"/>
-    <mergeCell ref="M151:N151"/>
-    <mergeCell ref="M152:N152"/>
-    <mergeCell ref="M153:N153"/>
-    <mergeCell ref="M154:N154"/>
-    <mergeCell ref="M155:N155"/>
-    <mergeCell ref="M135:N135"/>
-    <mergeCell ref="M136:N136"/>
-    <mergeCell ref="M137:N137"/>
-    <mergeCell ref="M148:N148"/>
-    <mergeCell ref="M138:N138"/>
-    <mergeCell ref="M144:N144"/>
-    <mergeCell ref="M162:N162"/>
-    <mergeCell ref="M173:N173"/>
-    <mergeCell ref="M174:N174"/>
-    <mergeCell ref="M156:N156"/>
-    <mergeCell ref="M157:N157"/>
-    <mergeCell ref="M158:N158"/>
-    <mergeCell ref="M159:N159"/>
-    <mergeCell ref="M160:N160"/>
-    <mergeCell ref="M161:N161"/>
-    <mergeCell ref="M191:N191"/>
-    <mergeCell ref="M192:N192"/>
-    <mergeCell ref="M197:N197"/>
-    <mergeCell ref="M180:N180"/>
-    <mergeCell ref="M181:N181"/>
-    <mergeCell ref="M182:N182"/>
-    <mergeCell ref="M183:N183"/>
-    <mergeCell ref="M184:N184"/>
-    <mergeCell ref="M185:N185"/>
+    <mergeCell ref="M383:N383"/>
+    <mergeCell ref="M384:N384"/>
+    <mergeCell ref="M387:N387"/>
+    <mergeCell ref="M371:N371"/>
+    <mergeCell ref="M372:N372"/>
+    <mergeCell ref="M373:N373"/>
+    <mergeCell ref="M378:N378"/>
+    <mergeCell ref="M379:N379"/>
+    <mergeCell ref="M380:N380"/>
+    <mergeCell ref="M361:N361"/>
+    <mergeCell ref="M362:N362"/>
+    <mergeCell ref="M363:N363"/>
+    <mergeCell ref="M367:N367"/>
+    <mergeCell ref="M368:N368"/>
+    <mergeCell ref="M369:N369"/>
+    <mergeCell ref="M354:N354"/>
+    <mergeCell ref="M355:N355"/>
+    <mergeCell ref="M356:N356"/>
+    <mergeCell ref="M357:N357"/>
+    <mergeCell ref="M359:N359"/>
+    <mergeCell ref="M360:N360"/>
+    <mergeCell ref="M351:N351"/>
+    <mergeCell ref="M352:N352"/>
+    <mergeCell ref="M353:N353"/>
+    <mergeCell ref="M329:N329"/>
+    <mergeCell ref="M332:N332"/>
+    <mergeCell ref="M336:N336"/>
+    <mergeCell ref="M337:N337"/>
+    <mergeCell ref="M342:N342"/>
+    <mergeCell ref="M350:N350"/>
+    <mergeCell ref="M321:N321"/>
+    <mergeCell ref="M322:N322"/>
+    <mergeCell ref="M325:N325"/>
+    <mergeCell ref="M326:N326"/>
+    <mergeCell ref="M327:N327"/>
+    <mergeCell ref="M328:N328"/>
+    <mergeCell ref="M312:N312"/>
+    <mergeCell ref="M313:N313"/>
+    <mergeCell ref="M314:N314"/>
+    <mergeCell ref="M315:N315"/>
+    <mergeCell ref="M317:N317"/>
+    <mergeCell ref="M318:N318"/>
+    <mergeCell ref="M298:N298"/>
+    <mergeCell ref="M300:N300"/>
+    <mergeCell ref="M301:N301"/>
+    <mergeCell ref="M302:N302"/>
+    <mergeCell ref="M310:N310"/>
+    <mergeCell ref="M311:N311"/>
+    <mergeCell ref="M289:N289"/>
+    <mergeCell ref="M290:N290"/>
+    <mergeCell ref="M294:N294"/>
+    <mergeCell ref="M295:N295"/>
+    <mergeCell ref="M296:N296"/>
+    <mergeCell ref="M297:N297"/>
+    <mergeCell ref="M266:N266"/>
+    <mergeCell ref="M267:N267"/>
+    <mergeCell ref="M269:N269"/>
+    <mergeCell ref="M274:N274"/>
+    <mergeCell ref="M286:N286"/>
+    <mergeCell ref="M288:N288"/>
+    <mergeCell ref="M256:N256"/>
+    <mergeCell ref="M259:N259"/>
+    <mergeCell ref="M262:N262"/>
+    <mergeCell ref="M263:N263"/>
+    <mergeCell ref="M264:N264"/>
+    <mergeCell ref="M265:N265"/>
+    <mergeCell ref="M238:N238"/>
+    <mergeCell ref="M246:N246"/>
+    <mergeCell ref="M253:N253"/>
+    <mergeCell ref="M254:N254"/>
+    <mergeCell ref="M255:N255"/>
+    <mergeCell ref="M149:N149"/>
+    <mergeCell ref="M163:N163"/>
+    <mergeCell ref="M187:N187"/>
+    <mergeCell ref="M193:N193"/>
+    <mergeCell ref="M198:N198"/>
+    <mergeCell ref="M235:N235"/>
+    <mergeCell ref="M236:N236"/>
+    <mergeCell ref="M210:N210"/>
+    <mergeCell ref="M217:N217"/>
+    <mergeCell ref="M218:N218"/>
+    <mergeCell ref="M224:N224"/>
+    <mergeCell ref="M211:N211"/>
+    <mergeCell ref="M219:N219"/>
+    <mergeCell ref="M201:N201"/>
+    <mergeCell ref="M202:N202"/>
+    <mergeCell ref="M203:N203"/>
+    <mergeCell ref="M205:N205"/>
+    <mergeCell ref="M207:N207"/>
     <mergeCell ref="M102:N102"/>
     <mergeCell ref="M111:N111"/>
     <mergeCell ref="M121:N121"/>
@@ -70858,95 +70853,99 @@
     <mergeCell ref="M225:N225"/>
     <mergeCell ref="M186:N186"/>
     <mergeCell ref="M176:N176"/>
-    <mergeCell ref="M238:N238"/>
-    <mergeCell ref="M246:N246"/>
-    <mergeCell ref="M253:N253"/>
-    <mergeCell ref="M254:N254"/>
-    <mergeCell ref="M255:N255"/>
-    <mergeCell ref="M149:N149"/>
-    <mergeCell ref="M163:N163"/>
-    <mergeCell ref="M187:N187"/>
-    <mergeCell ref="M193:N193"/>
-    <mergeCell ref="M198:N198"/>
-    <mergeCell ref="M235:N235"/>
-    <mergeCell ref="M236:N236"/>
-    <mergeCell ref="M210:N210"/>
-    <mergeCell ref="M217:N217"/>
-    <mergeCell ref="M218:N218"/>
-    <mergeCell ref="M224:N224"/>
-    <mergeCell ref="M211:N211"/>
-    <mergeCell ref="M219:N219"/>
-    <mergeCell ref="M201:N201"/>
-    <mergeCell ref="M202:N202"/>
-    <mergeCell ref="M203:N203"/>
-    <mergeCell ref="M205:N205"/>
-    <mergeCell ref="M207:N207"/>
-    <mergeCell ref="M266:N266"/>
-    <mergeCell ref="M267:N267"/>
-    <mergeCell ref="M269:N269"/>
-    <mergeCell ref="M274:N274"/>
-    <mergeCell ref="M286:N286"/>
-    <mergeCell ref="M288:N288"/>
-    <mergeCell ref="M256:N256"/>
-    <mergeCell ref="M259:N259"/>
-    <mergeCell ref="M262:N262"/>
-    <mergeCell ref="M263:N263"/>
-    <mergeCell ref="M264:N264"/>
-    <mergeCell ref="M265:N265"/>
-    <mergeCell ref="M298:N298"/>
-    <mergeCell ref="M300:N300"/>
-    <mergeCell ref="M301:N301"/>
-    <mergeCell ref="M302:N302"/>
-    <mergeCell ref="M310:N310"/>
-    <mergeCell ref="M311:N311"/>
-    <mergeCell ref="M289:N289"/>
-    <mergeCell ref="M290:N290"/>
-    <mergeCell ref="M294:N294"/>
-    <mergeCell ref="M295:N295"/>
-    <mergeCell ref="M296:N296"/>
-    <mergeCell ref="M297:N297"/>
-    <mergeCell ref="M321:N321"/>
-    <mergeCell ref="M322:N322"/>
-    <mergeCell ref="M325:N325"/>
-    <mergeCell ref="M326:N326"/>
-    <mergeCell ref="M327:N327"/>
-    <mergeCell ref="M328:N328"/>
-    <mergeCell ref="M312:N312"/>
-    <mergeCell ref="M313:N313"/>
-    <mergeCell ref="M314:N314"/>
-    <mergeCell ref="M315:N315"/>
-    <mergeCell ref="M317:N317"/>
-    <mergeCell ref="M318:N318"/>
-    <mergeCell ref="M351:N351"/>
-    <mergeCell ref="M352:N352"/>
-    <mergeCell ref="M353:N353"/>
-    <mergeCell ref="M329:N329"/>
-    <mergeCell ref="M332:N332"/>
-    <mergeCell ref="M336:N336"/>
-    <mergeCell ref="M337:N337"/>
-    <mergeCell ref="M342:N342"/>
-    <mergeCell ref="M350:N350"/>
-    <mergeCell ref="M361:N361"/>
-    <mergeCell ref="M362:N362"/>
-    <mergeCell ref="M363:N363"/>
-    <mergeCell ref="M367:N367"/>
-    <mergeCell ref="M368:N368"/>
-    <mergeCell ref="M369:N369"/>
-    <mergeCell ref="M354:N354"/>
-    <mergeCell ref="M355:N355"/>
-    <mergeCell ref="M356:N356"/>
-    <mergeCell ref="M357:N357"/>
-    <mergeCell ref="M359:N359"/>
-    <mergeCell ref="M360:N360"/>
-    <mergeCell ref="M383:N383"/>
-    <mergeCell ref="M384:N384"/>
-    <mergeCell ref="M387:N387"/>
-    <mergeCell ref="M371:N371"/>
-    <mergeCell ref="M372:N372"/>
-    <mergeCell ref="M373:N373"/>
-    <mergeCell ref="M378:N378"/>
-    <mergeCell ref="M379:N379"/>
-    <mergeCell ref="M380:N380"/>
+    <mergeCell ref="M191:N191"/>
+    <mergeCell ref="M192:N192"/>
+    <mergeCell ref="M197:N197"/>
+    <mergeCell ref="M180:N180"/>
+    <mergeCell ref="M181:N181"/>
+    <mergeCell ref="M182:N182"/>
+    <mergeCell ref="M183:N183"/>
+    <mergeCell ref="M184:N184"/>
+    <mergeCell ref="M185:N185"/>
+    <mergeCell ref="M162:N162"/>
+    <mergeCell ref="M173:N173"/>
+    <mergeCell ref="M174:N174"/>
+    <mergeCell ref="M156:N156"/>
+    <mergeCell ref="M157:N157"/>
+    <mergeCell ref="M158:N158"/>
+    <mergeCell ref="M159:N159"/>
+    <mergeCell ref="M160:N160"/>
+    <mergeCell ref="M161:N161"/>
+    <mergeCell ref="M151:N151"/>
+    <mergeCell ref="M152:N152"/>
+    <mergeCell ref="M153:N153"/>
+    <mergeCell ref="M154:N154"/>
+    <mergeCell ref="M155:N155"/>
+    <mergeCell ref="M135:N135"/>
+    <mergeCell ref="M136:N136"/>
+    <mergeCell ref="M137:N137"/>
+    <mergeCell ref="M148:N148"/>
+    <mergeCell ref="M138:N138"/>
+    <mergeCell ref="M144:N144"/>
+    <mergeCell ref="M127:N127"/>
+    <mergeCell ref="M128:N128"/>
+    <mergeCell ref="M129:N129"/>
+    <mergeCell ref="M133:N133"/>
+    <mergeCell ref="M134:N134"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="M119:N119"/>
+    <mergeCell ref="M120:N120"/>
+    <mergeCell ref="M126:N126"/>
+    <mergeCell ref="M110:N110"/>
+    <mergeCell ref="M114:N114"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="M109:N109"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="M98:N98"/>
+    <mergeCell ref="M99:N99"/>
+    <mergeCell ref="M100:N100"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="M89:N89"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="M79:N79"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="M58:N58"/>
+    <mergeCell ref="M59:N59"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="M651:N720 M388:N641 M722:N808">

</xml_diff>